<commit_message>
corrections to the BettingSimulator
</commit_message>
<xml_diff>
--- a/Writing/week3/week3.xlsx
+++ b/Writing/week3/week3.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/yashkarle/soccer-ds-stats/Writing/week3/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C2F0EE6E-9971-9B4B-BE1D-317BEBD075A3}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{450501F0-4AD5-164B-B2D3-B8CB41FC49B6}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="19040" activeTab="2" xr2:uid="{E93522CD-A16F-944B-B80D-1F57AE0445AA}"/>
   </bookViews>
@@ -1207,7 +1207,7 @@
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="64">
+  <cellXfs count="66">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
@@ -1346,6 +1346,12 @@
     </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="2" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Comma" xfId="2" builtinId="3"/>
@@ -3196,7 +3202,7 @@
   <dimension ref="B2:R46"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="L11" sqref="L11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -3682,10 +3688,7 @@
       </c>
     </row>
     <row r="34" spans="2:14">
-      <c r="N34">
-        <f>ABS(E13 - E12)</f>
-        <v>0.38850192840637154</v>
-      </c>
+      <c r="N34" s="64"/>
     </row>
     <row r="35" spans="2:14">
       <c r="F35" t="s">
@@ -3706,6 +3709,7 @@
       <c r="L35" s="1" t="s">
         <v>69</v>
       </c>
+      <c r="N35" s="65"/>
     </row>
     <row r="37" spans="2:14">
       <c r="B37" s="1" t="s">
@@ -3759,9 +3763,10 @@
       </c>
     </row>
   </sheetData>
-  <mergeCells count="2">
+  <mergeCells count="3">
     <mergeCell ref="F12:F13"/>
     <mergeCell ref="G12:G13"/>
+    <mergeCell ref="N34:N35"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>

</xml_diff>

<commit_message>
week 4 content and 360-scouting viz
</commit_message>
<xml_diff>
--- a/Writing/week3/week3.xlsx
+++ b/Writing/week3/week3.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/yashkarle/soccer-ds-stats/Writing/week3/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{450501F0-4AD5-164B-B2D3-B8CB41FC49B6}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC3C2116-2FA1-0046-BE49-DE94800B03CD}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="19040" activeTab="2" xr2:uid="{E93522CD-A16F-944B-B80D-1F57AE0445AA}"/>
+    <workbookView xWindow="20" yWindow="500" windowWidth="33600" windowHeight="19040" activeTab="7" xr2:uid="{E93522CD-A16F-944B-B80D-1F57AE0445AA}"/>
   </bookViews>
   <sheets>
     <sheet name="Comms" sheetId="11" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="316" uniqueCount="277">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="324" uniqueCount="285">
   <si>
     <t>Key stats</t>
   </si>
@@ -484,19 +484,6 @@
   </si>
   <si>
     <r>
-      <t xml:space="preserve">4) Player and Coach (playing style) </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FF00B050"/>
-        <rFont val="Calibri (Body)_x0000_"/>
-      </rPr>
-      <t>clustering using UMAP, GMM, DBSCAN</t>
-    </r>
-  </si>
-  <si>
-    <r>
       <t>5) Live match &lt;win/draw/lose&gt; probabilities based on real-time match data (</t>
     </r>
     <r>
@@ -933,9 +920,6 @@
     <t>6) Club/Team Valuation using key parameters that might change according to scenario/situation; "Wisdom of crowds" Transfermarkt</t>
   </si>
   <si>
-    <t>Transfers roundup</t>
-  </si>
-  <si>
     <t>Jenkins</t>
   </si>
   <si>
@@ -948,9 +932,6 @@
     <t>Week3 at CT</t>
   </si>
   <si>
-    <t>Ted Knuston</t>
-  </si>
-  <si>
     <t>These ideas should feed into ds-notes repo on a regular basis</t>
   </si>
   <si>
@@ -963,21 +944,12 @@
     <t>https://towardsdatascience.com/data-driven-evaluation-of-football-players-skills-c1df36d61a4e</t>
   </si>
   <si>
-    <t>Break last week - watching the Blues live at the bridge</t>
-  </si>
-  <si>
-    <t>Routine!</t>
-  </si>
-  <si>
     <t>We have a logo!</t>
   </si>
   <si>
     <t>Change in the domain name</t>
   </si>
   <si>
-    <t>Tweet every day of the week</t>
-  </si>
-  <si>
     <t>Share on Reddit</t>
   </si>
   <si>
@@ -996,9 +968,6 @@
     <t>xG timeline</t>
   </si>
   <si>
-    <t>https://twitter.com/mixedknuts</t>
-  </si>
-  <si>
     <t>Metrics used for defenders and midfielders</t>
   </si>
   <si>
@@ -1036,6 +1005,61 @@
   </si>
   <si>
     <t>StatSports</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>Mark Carey</t>
+  </si>
+  <si>
+    <t>Article about matching players with teams from a scouting perspective</t>
+  </si>
+  <si>
+    <t>Antonio Gagliardi - Italy</t>
+  </si>
+  <si>
+    <t>https://theathletic.com/3109106/2022/02/06/meet-antonio-gagliardi-pirlos-assistant-and-mancinis-lead-match-analyst-at-euro-2020/</t>
+  </si>
+  <si>
+    <t>"In modern football, a role is no longer a position, it’s a function.”</t>
+  </si>
+  <si>
+    <t>“We push the left-back up, tuck the other one in and we have three defenders.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">“Usually we build up in a three-plus-two,” Gagliardi explains.  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">We have two playmakers in Jorginho and Verratti, and two 10s in Insigne and Barella. </t>
+  </si>
+  <si>
+    <t>This box of four players in the middle often allowed us to outnumber Belgium in midfield.</t>
+  </si>
+  <si>
+    <t>lack of pressing specific stats // tracking data</t>
+  </si>
+  <si>
+    <t>gegenpresses</t>
+  </si>
+  <si>
+    <t>https://theathletic.com/3079854/2022/02/07/europes-elite-are-circling-raphinha-so-where-would-suit-him-if-he-does-leave/</t>
+  </si>
+  <si>
+    <t>Tweet with @@@</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">4) Player and Coach (playing style) </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF00B050"/>
+        <rFont val="Calibri (Body)_x0000_"/>
+      </rPr>
+      <t>clustering using {UMAP, GMM, DBSCAN}</t>
+    </r>
   </si>
 </sst>
 </file>
@@ -2479,47 +2503,37 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5B5068ED-902C-3546-B15E-0748BE44D916}">
-  <dimension ref="B2:B9"/>
+  <dimension ref="B4:B9"/>
   <sheetViews>
     <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <sheetData>
-    <row r="2" spans="2:2">
-      <c r="B2" t="s">
-        <v>252</v>
-      </c>
-    </row>
-    <row r="3" spans="2:2">
-      <c r="B3" t="s">
-        <v>253</v>
-      </c>
-    </row>
     <row r="4" spans="2:2">
       <c r="B4" t="s">
-        <v>255</v>
+        <v>250</v>
       </c>
     </row>
     <row r="5" spans="2:2">
       <c r="B5" t="s">
-        <v>254</v>
+        <v>249</v>
       </c>
     </row>
     <row r="7" spans="2:2">
       <c r="B7" t="s">
-        <v>256</v>
+        <v>283</v>
       </c>
     </row>
     <row r="8" spans="2:2">
       <c r="B8" t="s">
-        <v>257</v>
+        <v>251</v>
       </c>
     </row>
     <row r="9" spans="2:2">
       <c r="B9" s="11" t="s">
-        <v>258</v>
+        <v>252</v>
       </c>
     </row>
   </sheetData>
@@ -2580,7 +2594,7 @@
       <c r="F7" s="10"/>
       <c r="G7" s="10"/>
       <c r="J7" s="8" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="8" spans="1:17">
@@ -2613,11 +2627,11 @@
         <v>2</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="C10" s="2"/>
       <c r="J10" s="10" t="s">
-        <v>260</v>
+        <v>254</v>
       </c>
       <c r="N10" s="4"/>
       <c r="O10" s="4"/>
@@ -2630,13 +2644,13 @@
         <v>23</v>
       </c>
       <c r="F11" s="2" t="s">
+        <v>162</v>
+      </c>
+      <c r="G11" t="s">
         <v>163</v>
       </c>
-      <c r="G11" t="s">
-        <v>164</v>
-      </c>
       <c r="J11" s="10" t="s">
-        <v>261</v>
+        <v>255</v>
       </c>
       <c r="N11" s="3"/>
       <c r="O11" s="3"/>
@@ -2648,7 +2662,7 @@
         <v>50</v>
       </c>
       <c r="F12" s="50" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="G12" s="50"/>
       <c r="N12" s="3"/>
@@ -2658,19 +2672,19 @@
     </row>
     <row r="13" spans="1:17">
       <c r="B13" s="2" t="s">
-        <v>262</v>
+        <v>256</v>
       </c>
       <c r="E13" s="3" t="s">
+        <v>132</v>
+      </c>
+      <c r="F13" s="3" t="s">
         <v>133</v>
       </c>
-      <c r="F13" s="3" t="s">
+      <c r="G13" s="3" t="s">
         <v>134</v>
       </c>
-      <c r="G13" s="3" t="s">
+      <c r="H13" s="3" t="s">
         <v>135</v>
-      </c>
-      <c r="H13" s="3" t="s">
-        <v>136</v>
       </c>
       <c r="N13" s="3"/>
       <c r="O13" s="3"/>
@@ -2679,17 +2693,17 @@
     </row>
     <row r="14" spans="1:17">
       <c r="E14" s="3" t="s">
+        <v>136</v>
+      </c>
+      <c r="F14" s="50" t="s">
         <v>137</v>
-      </c>
-      <c r="F14" s="50" t="s">
-        <v>138</v>
       </c>
       <c r="G14" s="50"/>
       <c r="H14" s="3" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="J14" s="1" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="N14" s="3"/>
       <c r="O14" s="3"/>
@@ -2701,17 +2715,17 @@
         <v>1</v>
       </c>
       <c r="E15" s="30" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="F15" s="51" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="G15" s="51"/>
       <c r="H15" s="3" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="J15" s="26" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="N15" s="3"/>
       <c r="O15" s="3"/>
@@ -2726,7 +2740,7 @@
       <c r="F16" s="10"/>
       <c r="G16" s="10"/>
       <c r="J16" s="26" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="N16" s="3"/>
       <c r="O16" s="3"/>
@@ -2742,7 +2756,7 @@
       <c r="F17" s="10"/>
       <c r="G17" s="10"/>
       <c r="J17" s="11" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="N17" s="3"/>
       <c r="O17" s="3"/>
@@ -2754,7 +2768,7 @@
       <c r="C18" s="10"/>
       <c r="D18" s="10"/>
       <c r="J18" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="N18" s="3"/>
       <c r="O18" s="3"/>
@@ -2771,7 +2785,7 @@
       <c r="H19" s="10"/>
       <c r="I19" s="10"/>
       <c r="J19" s="11" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="K19" s="10"/>
       <c r="L19" s="10"/>
@@ -2796,7 +2810,7 @@
       <c r="H20" s="10"/>
       <c r="I20" s="10"/>
       <c r="J20" s="22" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="P20" s="10"/>
       <c r="Q20" s="10"/>
@@ -2813,7 +2827,7 @@
       <c r="H21" s="10"/>
       <c r="I21" s="10"/>
       <c r="J21" s="22" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="P21" s="10"/>
       <c r="Q21" s="10"/>
@@ -2830,7 +2844,7 @@
       <c r="H22" s="10"/>
       <c r="I22" s="10"/>
       <c r="J22" s="11" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="P22" s="10"/>
       <c r="Q22" s="10"/>
@@ -2847,7 +2861,7 @@
       <c r="H23" s="10"/>
       <c r="I23" s="10"/>
       <c r="J23" s="11" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="P23" s="10"/>
       <c r="Q23" s="10"/>
@@ -3201,8 +3215,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A82DF0DB-5968-4B43-A8AA-4F8D1A6A0F46}">
   <dimension ref="B2:R46"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="L11" sqref="L11"/>
+    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="Q26" sqref="Q26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -3253,7 +3267,7 @@
     </row>
     <row r="4" spans="2:18">
       <c r="B4" s="17" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="J4" s="3">
         <v>1.69</v>
@@ -3344,7 +3358,7 @@
         <v>0.19011406844106465</v>
       </c>
       <c r="N7" s="1" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="8" spans="2:18">
@@ -3565,12 +3579,12 @@
       </c>
       <c r="N26" s="2"/>
       <c r="O26" s="2"/>
-      <c r="Q26" t="s">
+      <c r="Q26" s="21" t="s">
         <v>102</v>
       </c>
     </row>
     <row r="27" spans="2:18">
-      <c r="C27" t="s">
+      <c r="C27" s="21" t="s">
         <v>75</v>
       </c>
       <c r="I27" s="1" t="s">
@@ -3624,7 +3638,7 @@
       </c>
     </row>
     <row r="30" spans="2:18">
-      <c r="C30" t="s">
+      <c r="C30" s="21" t="s">
         <v>77</v>
       </c>
       <c r="N30" s="19">
@@ -3656,7 +3670,7 @@
         <v>0.1905</v>
       </c>
       <c r="L31" s="1" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="32" spans="2:18">
@@ -3670,7 +3684,7 @@
         <v>0.17</v>
       </c>
       <c r="L32" s="1" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="33" spans="2:14">
@@ -3684,7 +3698,7 @@
         <v>0.12181139182480299</v>
       </c>
       <c r="L33" s="1" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="34" spans="2:14">
@@ -3692,7 +3706,7 @@
     </row>
     <row r="35" spans="2:14">
       <c r="F35" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="I35" s="28">
         <f>AVERAGE(I31:I33)</f>
@@ -3710,6 +3724,11 @@
         <v>69</v>
       </c>
       <c r="N35" s="65"/>
+    </row>
+    <row r="36" spans="2:14">
+      <c r="K36" t="s">
+        <v>270</v>
+      </c>
     </row>
     <row r="37" spans="2:14">
       <c r="B37" s="1" t="s">
@@ -3751,15 +3770,15 @@
     </row>
     <row r="45" spans="2:14">
       <c r="B45" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="C45" t="s">
         <v>128</v>
-      </c>
-      <c r="C45" t="s">
-        <v>129</v>
       </c>
     </row>
     <row r="46" spans="2:14">
       <c r="C46" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
   </sheetData>
@@ -3768,105 +3787,154 @@
     <mergeCell ref="G12:G13"/>
     <mergeCell ref="N34:N35"/>
   </mergeCells>
+  <hyperlinks>
+    <hyperlink ref="C27" r:id="rId1" xr:uid="{93283E62-74FB-A14D-AD7E-9C7971E1C757}"/>
+    <hyperlink ref="C30" r:id="rId2" xr:uid="{A3C1AED9-73BF-EB42-9CC0-99C38C03E075}"/>
+    <hyperlink ref="Q26" r:id="rId3" xr:uid="{4423A1C9-96FD-0046-9448-5923E62026CC}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
+  <drawing r:id="rId4"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F0964CF1-FDC5-0142-B968-561FCC0D04D5}">
-  <dimension ref="B2:H17"/>
+  <dimension ref="B2:L20"/>
   <sheetViews>
     <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="E16" sqref="E16"/>
+      <selection activeCell="J3" sqref="J3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <sheetData>
-    <row r="2" spans="2:8">
+    <row r="2" spans="2:12">
       <c r="B2" s="1" t="s">
         <v>7</v>
       </c>
       <c r="C2" s="10" t="s">
-        <v>247</v>
+        <v>271</v>
       </c>
       <c r="D2" s="10" t="s">
-        <v>263</v>
+        <v>272</v>
       </c>
       <c r="E2" s="10"/>
       <c r="F2" s="10"/>
       <c r="G2" s="10"/>
-    </row>
-    <row r="3" spans="2:8">
+      <c r="J2" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="3" spans="2:12">
       <c r="B3" s="1"/>
-      <c r="C3" s="10" t="s">
-        <v>266</v>
+      <c r="C3" s="2" t="s">
+        <v>259</v>
       </c>
       <c r="D3" s="10" t="s">
-        <v>267</v>
+        <v>260</v>
       </c>
       <c r="E3" s="10"/>
       <c r="F3" s="10"/>
       <c r="G3" s="10"/>
     </row>
-    <row r="5" spans="2:8">
+    <row r="5" spans="2:12">
       <c r="B5" s="1" t="s">
         <v>8</v>
       </c>
       <c r="C5" t="s">
-        <v>264</v>
+        <v>257</v>
       </c>
       <c r="G5" t="s">
-        <v>265</v>
-      </c>
-    </row>
-    <row r="7" spans="2:8">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="7" spans="2:12">
       <c r="B7" s="6" t="s">
         <v>27</v>
       </c>
       <c r="C7" s="6"/>
     </row>
-    <row r="8" spans="2:8">
+    <row r="8" spans="2:12">
       <c r="B8" s="7"/>
       <c r="C8" s="7" t="s">
-        <v>242</v>
-      </c>
-      <c r="F8" s="10"/>
+        <v>273</v>
+      </c>
+      <c r="F8" s="10" t="s">
+        <v>274</v>
+      </c>
       <c r="G8" s="10"/>
       <c r="H8" s="10"/>
     </row>
-    <row r="9" spans="2:8">
+    <row r="9" spans="2:12">
       <c r="B9" s="7"/>
       <c r="C9" s="7"/>
-    </row>
-    <row r="11" spans="2:8">
-      <c r="B11" s="1" t="s">
+      <c r="F9" s="10" t="s">
+        <v>275</v>
+      </c>
+      <c r="G9" s="10"/>
+      <c r="H9" s="10"/>
+      <c r="L9" t="s">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="10" spans="2:12">
+      <c r="B10" s="7"/>
+      <c r="C10" s="7"/>
+      <c r="F10" s="10" t="s">
+        <v>280</v>
+      </c>
+      <c r="G10" s="10"/>
+      <c r="H10" s="10"/>
+      <c r="L10" t="s">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="11" spans="2:12">
+      <c r="B11" s="7"/>
+      <c r="C11" s="7"/>
+      <c r="F11" s="10" t="s">
+        <v>281</v>
+      </c>
+      <c r="G11" s="10"/>
+      <c r="H11" s="10"/>
+      <c r="L11" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="12" spans="2:12">
+      <c r="B12" s="7"/>
+      <c r="C12" s="7"/>
+      <c r="L12" t="s">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="14" spans="2:12">
+      <c r="B14" s="1" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="16" spans="2:12">
+      <c r="D16" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="13" spans="2:8">
-      <c r="D13" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="14" spans="2:8">
-      <c r="D14" t="s">
+    <row r="17" spans="4:5">
+      <c r="D17" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="18" spans="4:5">
+      <c r="E18" t="s">
         <v>175</v>
       </c>
     </row>
-    <row r="15" spans="2:8">
-      <c r="E15" t="s">
+    <row r="19" spans="4:5">
+      <c r="E19" t="s">
         <v>176</v>
       </c>
     </row>
-    <row r="16" spans="2:8">
-      <c r="E16" t="s">
+    <row r="20" spans="4:5">
+      <c r="E20" t="s">
         <v>177</v>
-      </c>
-    </row>
-    <row r="17" spans="5:5">
-      <c r="E17" t="s">
-        <v>178</v>
       </c>
     </row>
   </sheetData>
@@ -3889,10 +3957,10 @@
   <sheetData>
     <row r="1" spans="1:9">
       <c r="A1" s="1" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="F1" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
     </row>
     <row r="2" spans="1:9">
@@ -3900,7 +3968,7 @@
         <v>4</v>
       </c>
       <c r="F2" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
     </row>
     <row r="3" spans="1:9">
@@ -3911,7 +3979,7 @@
         <v>56</v>
       </c>
       <c r="G3" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="H3" t="s">
         <v>38</v>
@@ -3922,7 +3990,7 @@
         <v>22</v>
       </c>
       <c r="G4" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="H4" t="s">
         <v>39</v>
@@ -3930,7 +3998,7 @@
     </row>
     <row r="5" spans="1:9">
       <c r="G5" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="H5" t="s">
         <v>40</v>
@@ -3941,7 +4009,7 @@
         <v>18</v>
       </c>
       <c r="H6" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="I6" t="s">
         <v>41</v>
@@ -3952,7 +4020,7 @@
         <v>19</v>
       </c>
       <c r="H7" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="I7" t="s">
         <v>42</v>
@@ -3963,7 +4031,7 @@
         <v>20</v>
       </c>
       <c r="H8" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="I8" t="s">
         <v>43</v>
@@ -3977,7 +4045,7 @@
         <v>31</v>
       </c>
       <c r="I9" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="10" spans="1:9">
@@ -3993,17 +4061,17 @@
     </row>
     <row r="14" spans="1:9">
       <c r="B14" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="15" spans="1:9">
       <c r="B15" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="17" spans="2:2">
       <c r="B17" t="s">
-        <v>269</v>
+        <v>262</v>
       </c>
     </row>
   </sheetData>
@@ -4019,8 +4087,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F9E2E5E7-DDB3-A142-A108-0A0B629951B0}">
   <dimension ref="A2:O38"/>
   <sheetViews>
-    <sheetView topLeftCell="A5" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="G33" sqref="G33"/>
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="M23" sqref="M23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -4045,10 +4113,10 @@
         <v>26</v>
       </c>
       <c r="B4" s="11" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="G4" s="11" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
     </row>
     <row r="5" spans="1:12">
@@ -4057,7 +4125,7 @@
         <v>56</v>
       </c>
       <c r="H5" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
     </row>
     <row r="6" spans="1:12">
@@ -4068,29 +4136,29 @@
         <v>28</v>
       </c>
       <c r="H6" s="7" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="I6" s="7" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
     </row>
     <row r="7" spans="1:12">
       <c r="C7" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="H7" s="7" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="I7" s="7" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
     </row>
     <row r="8" spans="1:12">
       <c r="C8" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
     </row>
     <row r="9" spans="1:12">
@@ -4098,7 +4166,7 @@
         <v>15</v>
       </c>
       <c r="H9" s="7" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
     </row>
     <row r="10" spans="1:12">
@@ -4108,43 +4176,43 @@
     </row>
     <row r="11" spans="1:12">
       <c r="C11" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="G11" t="s">
+        <v>197</v>
+      </c>
+      <c r="H11" t="s">
         <v>198</v>
-      </c>
-      <c r="H11" t="s">
-        <v>199</v>
       </c>
     </row>
     <row r="12" spans="1:12">
       <c r="C12" t="s">
-        <v>268</v>
+        <v>261</v>
       </c>
       <c r="G12" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
     </row>
     <row r="14" spans="1:12">
       <c r="G14" s="26" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
     </row>
     <row r="15" spans="1:12">
       <c r="E15" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="F15">
         <v>1</v>
       </c>
       <c r="G15" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="J15" s="2">
         <v>0.05</v>
       </c>
       <c r="K15" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="L15">
         <v>0.95</v>
@@ -4155,13 +4223,13 @@
         <v>2</v>
       </c>
       <c r="G16" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="J16" s="2">
         <v>0.05</v>
       </c>
       <c r="K16" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="L16">
         <v>0.95</v>
@@ -4169,12 +4237,12 @@
     </row>
     <row r="18" spans="6:15">
       <c r="G18" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
     </row>
     <row r="19" spans="6:15">
       <c r="G19" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="O19" s="2">
         <v>0.01</v>
@@ -4182,12 +4250,12 @@
     </row>
     <row r="20" spans="6:15">
       <c r="G20" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
     </row>
     <row r="22" spans="6:15">
       <c r="G22" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="J22" s="47">
         <v>10000000</v>
@@ -4195,41 +4263,41 @@
     </row>
     <row r="23" spans="6:15">
       <c r="G23" s="1" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
     </row>
     <row r="24" spans="6:15">
       <c r="G24" t="s">
+        <v>212</v>
+      </c>
+      <c r="H24" t="s">
         <v>213</v>
       </c>
-      <c r="H24" t="s">
+      <c r="I24" t="s">
         <v>214</v>
       </c>
-      <c r="I24" t="s">
+      <c r="J24" t="s">
         <v>215</v>
       </c>
-      <c r="J24" t="s">
+      <c r="K24" t="s">
         <v>216</v>
-      </c>
-      <c r="K24" t="s">
-        <v>217</v>
       </c>
     </row>
     <row r="25" spans="6:15">
       <c r="F25" s="3" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="G25" s="3" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="H25" s="3" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="I25" s="3" t="s">
+        <v>224</v>
+      </c>
+      <c r="J25" s="3" t="s">
         <v>225</v>
-      </c>
-      <c r="J25" s="3" t="s">
-        <v>226</v>
       </c>
       <c r="K25" s="3">
         <v>0.999</v>
@@ -4237,19 +4305,19 @@
     </row>
     <row r="26" spans="6:15">
       <c r="F26" s="3" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="G26" s="3" t="s">
+        <v>217</v>
+      </c>
+      <c r="H26" s="3" t="s">
         <v>218</v>
       </c>
-      <c r="H26" s="3" t="s">
-        <v>219</v>
-      </c>
       <c r="I26" s="3" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="J26" s="3" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="K26" s="3">
         <v>0.84</v>
@@ -4257,19 +4325,19 @@
     </row>
     <row r="27" spans="6:15">
       <c r="F27" s="3" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="G27" s="3" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="H27" s="3" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="I27" s="3" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="J27" s="3" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="K27" s="3">
         <v>5.1999999999999995E-4</v>
@@ -4277,19 +4345,19 @@
     </row>
     <row r="28" spans="6:15">
       <c r="F28" s="29" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="G28" s="29" t="s">
+        <v>218</v>
+      </c>
+      <c r="H28" s="29" t="s">
         <v>219</v>
       </c>
-      <c r="H28" s="29" t="s">
-        <v>220</v>
-      </c>
       <c r="I28" s="29" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="J28" s="29" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="K28" s="29">
         <v>0.16</v>
@@ -4297,55 +4365,55 @@
     </row>
     <row r="29" spans="6:15">
       <c r="G29" s="26" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
     </row>
     <row r="31" spans="6:15">
       <c r="G31" s="48" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
     </row>
     <row r="32" spans="6:15">
       <c r="G32" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
     </row>
     <row r="33" spans="6:11">
       <c r="G33" s="48" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
     </row>
     <row r="35" spans="6:11">
       <c r="G35" s="17" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
     </row>
     <row r="36" spans="6:11">
       <c r="F36" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="G36" s="49" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="H36" s="10"/>
       <c r="I36" s="49" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="J36" s="49" t="s">
+        <v>238</v>
+      </c>
+      <c r="K36" s="49" t="s">
         <v>239</v>
-      </c>
-      <c r="K36" s="49" t="s">
-        <v>240</v>
       </c>
     </row>
     <row r="37" spans="6:11">
       <c r="G37" s="17" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
     </row>
     <row r="38" spans="6:11">
       <c r="G38" s="17" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
     </row>
   </sheetData>
@@ -4375,24 +4443,24 @@
         <v>9</v>
       </c>
       <c r="C2" t="s">
-        <v>272</v>
+        <v>265</v>
       </c>
       <c r="E2" s="21"/>
     </row>
     <row r="3" spans="2:5">
       <c r="B3" s="1"/>
       <c r="C3" t="s">
-        <v>249</v>
+        <v>246</v>
       </c>
       <c r="E3" s="21"/>
     </row>
     <row r="4" spans="2:5">
       <c r="B4" s="1"/>
       <c r="C4" t="s">
-        <v>276</v>
+        <v>269</v>
       </c>
       <c r="D4" s="21" t="s">
-        <v>250</v>
+        <v>247</v>
       </c>
       <c r="E4" s="21"/>
     </row>
@@ -4412,7 +4480,7 @@
     <row r="8" spans="2:5">
       <c r="B8" s="1"/>
       <c r="C8" t="s">
-        <v>271</v>
+        <v>264</v>
       </c>
     </row>
     <row r="10" spans="2:5">
@@ -4426,7 +4494,7 @@
     <row r="11" spans="2:5">
       <c r="B11" s="62"/>
       <c r="C11" s="11" t="s">
-        <v>270</v>
+        <v>263</v>
       </c>
     </row>
     <row r="12" spans="2:5">
@@ -4438,22 +4506,22 @@
         <v>12</v>
       </c>
       <c r="C13" t="s">
+        <v>116</v>
+      </c>
+      <c r="E13" t="s">
         <v>117</v>
-      </c>
-      <c r="E13" t="s">
-        <v>118</v>
       </c>
     </row>
     <row r="14" spans="2:5">
       <c r="B14" s="1"/>
       <c r="C14" s="63" t="s">
-        <v>273</v>
+        <v>266</v>
       </c>
     </row>
     <row r="15" spans="2:5">
       <c r="B15" s="1"/>
       <c r="C15" s="63" t="s">
-        <v>275</v>
+        <v>268</v>
       </c>
     </row>
     <row r="17" spans="2:3">
@@ -4469,7 +4537,7 @@
         <v>14</v>
       </c>
       <c r="C18" t="s">
-        <v>274</v>
+        <v>267</v>
       </c>
     </row>
   </sheetData>
@@ -4481,8 +4549,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6476FE99-38C7-4044-A99D-0C60D07A6712}">
   <dimension ref="A1:K35"/>
   <sheetViews>
-    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -4501,7 +4569,7 @@
         <v>32</v>
       </c>
       <c r="B1" t="s">
-        <v>248</v>
+        <v>245</v>
       </c>
     </row>
     <row r="2" spans="1:11">
@@ -4509,7 +4577,7 @@
         <v>110</v>
       </c>
       <c r="C2" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="3" spans="1:11">
@@ -4518,7 +4586,7 @@
         <v>112</v>
       </c>
       <c r="C3" t="s">
-        <v>251</v>
+        <v>248</v>
       </c>
       <c r="G3" s="11"/>
       <c r="H3" s="10"/>
@@ -4536,7 +4604,7 @@
     </row>
     <row r="5" spans="1:11">
       <c r="B5" s="10" t="s">
-        <v>113</v>
+        <v>284</v>
       </c>
       <c r="H5" s="10"/>
       <c r="I5" s="52"/>
@@ -4546,17 +4614,17 @@
     <row r="6" spans="1:11">
       <c r="A6" s="9"/>
       <c r="B6" s="10" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="C6" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="H6" s="10"/>
     </row>
     <row r="7" spans="1:11">
       <c r="A7" s="9"/>
       <c r="B7" s="10" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="H7" s="10"/>
     </row>
@@ -4585,37 +4653,37 @@
     </row>
     <row r="13" spans="1:11">
       <c r="B13" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
     </row>
     <row r="16" spans="1:11">
       <c r="A16" s="1" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="18" spans="2:8">
       <c r="B18" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
     </row>
     <row r="19" spans="2:8">
       <c r="B19" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
     </row>
     <row r="20" spans="2:8">
       <c r="B20" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="21" spans="2:8">
       <c r="B21" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
     </row>
     <row r="24" spans="2:8">
       <c r="B24" s="61" t="s">
-        <v>259</v>
+        <v>253</v>
       </c>
       <c r="C24" s="7"/>
       <c r="D24" s="7"/>
@@ -4625,7 +4693,7 @@
     </row>
     <row r="25" spans="2:8">
       <c r="C25" s="6" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="D25" s="7"/>
       <c r="E25" s="7"/>
@@ -4641,33 +4709,33 @@
         <v>2</v>
       </c>
       <c r="E26" s="56" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="F26" s="56" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="G26" s="56" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="H26" s="56" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="27" spans="2:8">
       <c r="C27" s="42" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="D27" s="42" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="E27" s="42" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="F27" s="42" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="G27" s="42" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="H27" s="42">
         <v>0</v>
@@ -4675,17 +4743,17 @@
     </row>
     <row r="28" spans="2:8">
       <c r="C28" s="42" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="D28" s="42"/>
       <c r="E28" s="42" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="F28" s="42" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="G28" s="42" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="H28" s="42">
         <v>1</v>
@@ -4693,17 +4761,17 @@
     </row>
     <row r="29" spans="2:8">
       <c r="C29" s="42" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="D29" s="42"/>
       <c r="E29" s="42" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="F29" s="42" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="G29" s="42" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="H29" s="42">
         <v>0</v>
@@ -4711,17 +4779,17 @@
     </row>
     <row r="30" spans="2:8">
       <c r="C30" s="57" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="D30" s="57"/>
       <c r="E30" s="57" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="F30" s="57" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="G30" s="57" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="H30" s="57">
         <v>0</v>
@@ -4731,13 +4799,13 @@
       <c r="C31" s="42"/>
       <c r="D31" s="42"/>
       <c r="E31" s="42" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="F31" s="42" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="G31" s="58" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="H31" s="42">
         <v>0</v>
@@ -4747,13 +4815,13 @@
       <c r="C32" s="42"/>
       <c r="D32" s="42"/>
       <c r="E32" s="42" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="F32" s="42" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="G32" s="59" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="H32" s="42">
         <v>0</v>
@@ -4763,13 +4831,13 @@
       <c r="C33" s="42"/>
       <c r="D33" s="42"/>
       <c r="E33" s="42" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="F33" s="42" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="G33" s="60" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="H33" s="42">
         <v>0</v>
@@ -4777,17 +4845,17 @@
     </row>
     <row r="34" spans="3:8">
       <c r="C34" s="42" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="D34" s="42"/>
       <c r="E34" s="42" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="F34" s="42" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="G34" s="59" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="H34" s="42">
         <v>0</v>
@@ -4797,13 +4865,13 @@
       <c r="C35" s="7"/>
       <c r="D35" s="7"/>
       <c r="E35" s="42" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="F35" s="42" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="G35" s="59" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="H35" s="42">
         <v>0</v>

</xml_diff>